<commit_message>
updated code a bit
</commit_message>
<xml_diff>
--- a/raw_data/arthropods.xlsx
+++ b/raw_data/arthropods.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8786" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8786" uniqueCount="489">
   <si>
     <t>Region</t>
   </si>
@@ -1143,9 +1143,6 @@
   </si>
   <si>
     <t>Cryptoglossa</t>
-  </si>
-  <si>
-    <t>CA 101?</t>
   </si>
   <si>
     <t>Forelius mccooki</t>
@@ -2473,9 +2470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1062"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K92" sqref="K92"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A623" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L730" sqref="L730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2618,10 +2615,10 @@
         <v>228</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N3" s="7">
         <v>1</v>
@@ -2931,7 +2928,7 @@
         <v>67</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N11" s="7">
         <v>1</v>
@@ -3007,7 +3004,7 @@
         <v>70</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>70</v>
@@ -3125,10 +3122,10 @@
         <v>95</v>
       </c>
       <c r="L16" s="51" t="s">
+        <v>431</v>
+      </c>
+      <c r="M16" s="51" t="s">
         <v>432</v>
-      </c>
-      <c r="M16" s="51" t="s">
-        <v>433</v>
       </c>
       <c r="N16" s="51"/>
       <c r="O16" s="51"/>
@@ -3243,10 +3240,10 @@
         <v>276</v>
       </c>
       <c r="L19" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="M19" s="26" t="s">
         <v>474</v>
-      </c>
-      <c r="M19" s="26" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -3318,17 +3315,17 @@
         <v>270</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J21" s="26"/>
       <c r="K21" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="L21" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="L21" s="26" t="s">
-        <v>442</v>
-      </c>
       <c r="M21" s="26" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
@@ -3404,17 +3401,17 @@
         <v>15</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J23" s="36"/>
       <c r="K23" s="36" t="s">
+        <v>443</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="M23" s="36" t="s">
         <v>444</v>
-      </c>
-      <c r="L23" s="36" t="s">
-        <v>420</v>
-      </c>
-      <c r="M23" s="36" t="s">
-        <v>445</v>
       </c>
       <c r="N23" s="7">
         <v>2</v>
@@ -3453,10 +3450,10 @@
         <v>256</v>
       </c>
       <c r="L24" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="M24" s="7" t="s">
         <v>460</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>461</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -3491,13 +3488,13 @@
         <v>52</v>
       </c>
       <c r="I25" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -3578,10 +3575,10 @@
         <v>14</v>
       </c>
       <c r="K27" s="44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="M27" s="44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N27" s="51">
         <v>12</v>
@@ -3616,17 +3613,17 @@
         <v>15</v>
       </c>
       <c r="I28" s="36" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J28" s="26"/>
       <c r="K28" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="L28" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="M28" s="26" t="s">
         <v>444</v>
-      </c>
-      <c r="L28" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="M28" s="26" t="s">
-        <v>445</v>
       </c>
       <c r="N28" s="26"/>
       <c r="O28" s="26"/>
@@ -3741,13 +3738,13 @@
         <v>105</v>
       </c>
       <c r="L31" s="26" t="s">
+        <v>436</v>
+      </c>
+      <c r="M31" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="M31" s="26" t="s">
-        <v>438</v>
-      </c>
       <c r="O31" s="26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P31" s="26"/>
       <c r="Q31" s="26"/>
@@ -3864,10 +3861,10 @@
         <v>280</v>
       </c>
       <c r="L34" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="M34" s="35" t="s">
         <v>427</v>
-      </c>
-      <c r="M34" s="35" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -3985,10 +3982,10 @@
         <v>112</v>
       </c>
       <c r="L37" s="36" t="s">
+        <v>428</v>
+      </c>
+      <c r="M37" s="35" t="s">
         <v>429</v>
-      </c>
-      <c r="M37" s="35" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.35">
@@ -4229,11 +4226,11 @@
       </c>
       <c r="J43" s="26"/>
       <c r="K43" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L43" s="26"/>
       <c r="M43" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N43" s="26">
         <v>1</v>
@@ -4360,10 +4357,10 @@
         <v>73</v>
       </c>
       <c r="L46" s="50" t="s">
+        <v>388</v>
+      </c>
+      <c r="M46" s="39" t="s">
         <v>389</v>
-      </c>
-      <c r="M46" s="39" t="s">
-        <v>390</v>
       </c>
       <c r="N46" s="39"/>
       <c r="O46" s="39" t="s">
@@ -4441,17 +4438,17 @@
         <v>30</v>
       </c>
       <c r="I48" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="J48" s="50" t="s">
         <v>423</v>
       </c>
-      <c r="J48" s="50" t="s">
-        <v>424</v>
-      </c>
       <c r="K48" s="50" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L48" s="50"/>
       <c r="M48" s="50" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="N48" s="50"/>
       <c r="O48" s="50" t="s">
@@ -4486,15 +4483,15 @@
         <v>25</v>
       </c>
       <c r="I49" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J49" s="39"/>
       <c r="K49" s="50" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L49" s="39"/>
       <c r="M49" s="39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="N49" s="39">
         <v>1</v>
@@ -4625,11 +4622,11 @@
       </c>
       <c r="J52" s="60"/>
       <c r="K52" s="60" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L52" s="60"/>
       <c r="M52" s="60" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N52" s="60">
         <v>1</v>
@@ -4745,10 +4742,10 @@
         <v>330</v>
       </c>
       <c r="L55" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="M55" s="7" t="s">
         <v>458</v>
-      </c>
-      <c r="M55" s="7" t="s">
-        <v>459</v>
       </c>
       <c r="N55" s="7">
         <v>4</v>
@@ -4976,13 +4973,13 @@
         <v>14</v>
       </c>
       <c r="K61" s="51" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L61" s="51" t="s">
+        <v>476</v>
+      </c>
+      <c r="M61" s="51" t="s">
         <v>477</v>
-      </c>
-      <c r="M61" s="51" t="s">
-        <v>478</v>
       </c>
       <c r="N61" s="51">
         <v>11</v>
@@ -5017,10 +5014,10 @@
         <v>31</v>
       </c>
       <c r="K62" s="36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="M62" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="N62" s="7">
         <v>4</v>
@@ -5058,10 +5055,10 @@
         <v>73</v>
       </c>
       <c r="L63" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M63" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M63" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="64" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -5131,10 +5128,10 @@
         <v>256</v>
       </c>
       <c r="L65" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="M65" s="7" t="s">
         <v>463</v>
-      </c>
-      <c r="M65" s="7" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -5458,10 +5455,10 @@
         <v>280</v>
       </c>
       <c r="L74" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="M74" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="M74" s="7" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -5642,16 +5639,16 @@
         <v>134</v>
       </c>
       <c r="J79" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="K79" s="36" t="s">
         <v>448</v>
       </c>
-      <c r="K79" s="36" t="s">
+      <c r="L79" s="36" t="s">
         <v>449</v>
       </c>
-      <c r="L79" s="36" t="s">
+      <c r="M79" s="7" t="s">
         <v>450</v>
-      </c>
-      <c r="M79" s="7" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="80" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -5770,10 +5767,10 @@
         <v>280</v>
       </c>
       <c r="L82" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="M82" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="M82" s="7" t="s">
-        <v>428</v>
       </c>
       <c r="O82" s="26"/>
       <c r="P82" s="26"/>
@@ -5895,7 +5892,7 @@
       </c>
       <c r="J85" s="26"/>
       <c r="K85" s="26" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L85" s="26"/>
       <c r="M85" s="26" t="s">
@@ -6051,7 +6048,7 @@
         <v>133</v>
       </c>
       <c r="L89" s="36" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M89" s="36" t="s">
         <v>349</v>
@@ -6168,10 +6165,10 @@
         <v>256</v>
       </c>
       <c r="L92" s="36" t="s">
+        <v>459</v>
+      </c>
+      <c r="M92" s="36" t="s">
         <v>460</v>
-      </c>
-      <c r="M92" s="36" t="s">
-        <v>461</v>
       </c>
       <c r="N92" s="35">
         <v>1</v>
@@ -6244,13 +6241,13 @@
         <v>53</v>
       </c>
       <c r="K94" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L94" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="M94" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N94" s="36">
         <v>4</v>
@@ -6332,7 +6329,7 @@
         <v>318</v>
       </c>
       <c r="M96" s="51" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N96" s="51">
         <v>1</v>
@@ -6481,10 +6478,10 @@
         <v>73</v>
       </c>
       <c r="L100" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M100" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M100" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="101" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -6592,7 +6589,7 @@
         <v>153</v>
       </c>
       <c r="L103" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M103" s="7" t="s">
         <v>153</v>
@@ -6671,10 +6668,10 @@
         <v>105</v>
       </c>
       <c r="L105" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="M105" s="7" t="s">
         <v>437</v>
-      </c>
-      <c r="M105" s="7" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="51" customFormat="1" x14ac:dyDescent="0.35">
@@ -6823,10 +6820,10 @@
         <v>73</v>
       </c>
       <c r="L109" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M109" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M109" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -6928,13 +6925,13 @@
         <v>30</v>
       </c>
       <c r="I112" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="J112" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="J112" s="5" t="s">
-        <v>424</v>
-      </c>
       <c r="M112" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O112" s="5" t="s">
         <v>171</v>
@@ -7010,10 +7007,10 @@
         <v>105</v>
       </c>
       <c r="L114" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="M114" s="7" t="s">
         <v>437</v>
-      </c>
-      <c r="M114" s="7" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -7048,10 +7045,10 @@
         <v>173</v>
       </c>
       <c r="L115" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="M115" s="7" t="s">
         <v>399</v>
-      </c>
-      <c r="M115" s="7" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -7129,10 +7126,10 @@
         <v>302</v>
       </c>
       <c r="L117" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="M117" s="7" t="s">
         <v>373</v>
-      </c>
-      <c r="M117" s="7" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7203,10 +7200,10 @@
         <v>53</v>
       </c>
       <c r="K119" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M119" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N119" s="7">
         <v>1</v>
@@ -7282,47 +7279,47 @@
         <v>134</v>
       </c>
       <c r="K121" s="36" t="s">
+        <v>448</v>
+      </c>
+      <c r="L121" s="36" t="s">
         <v>449</v>
       </c>
-      <c r="L121" s="36" t="s">
+      <c r="M121" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="M121" s="7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="122" spans="1:17" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="27">
+    </row>
+    <row r="122" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="36">
         <v>286</v>
       </c>
-      <c r="B122" s="27" t="s">
+      <c r="B122" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C122" s="71" t="s">
+      <c r="C122" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="D122" s="45" t="s">
+      <c r="D122" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="E122" s="46">
+      <c r="E122" s="49">
         <v>2</v>
       </c>
-      <c r="F122" s="47" t="s">
+      <c r="F122" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="G122" s="27">
+      <c r="G122" s="36">
         <v>19</v>
       </c>
-      <c r="H122" s="27" t="s">
+      <c r="H122" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="I122" s="27" t="s">
+      <c r="I122" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="M122" s="27" t="s">
+      <c r="M122" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="N122" s="27">
+      <c r="N122" s="36">
         <v>1</v>
       </c>
     </row>
@@ -7393,10 +7390,10 @@
         <v>73</v>
       </c>
       <c r="L124" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M124" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M124" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="125" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -7431,10 +7428,10 @@
         <v>73</v>
       </c>
       <c r="L125" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M125" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M125" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -8494,10 +8491,10 @@
         <v>73</v>
       </c>
       <c r="L154" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M154" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M154" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="155" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -8757,10 +8754,10 @@
         <v>326</v>
       </c>
       <c r="L161" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="M161" s="7" t="s">
         <v>467</v>
-      </c>
-      <c r="M161" s="7" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="162" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -9030,11 +9027,11 @@
       </c>
       <c r="J168" s="26"/>
       <c r="K168" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L168" s="26"/>
       <c r="M168" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N168" s="26">
         <v>1</v>
@@ -9188,7 +9185,7 @@
         <v>132</v>
       </c>
       <c r="J172" s="26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K172" s="26"/>
       <c r="L172" s="26"/>
@@ -9378,10 +9375,10 @@
         <v>73</v>
       </c>
       <c r="L177" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M177" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M177" s="7" t="s">
-        <v>390</v>
       </c>
       <c r="O177" s="7">
         <v>1</v>
@@ -9661,10 +9658,10 @@
         <v>73</v>
       </c>
       <c r="L184" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="M184" s="28" t="s">
         <v>389</v>
-      </c>
-      <c r="M184" s="28" t="s">
-        <v>390</v>
       </c>
       <c r="N184" s="28"/>
       <c r="O184" s="28"/>
@@ -9704,7 +9701,7 @@
         <v>16</v>
       </c>
       <c r="L185" s="26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M185" s="26" t="s">
         <v>16</v>
@@ -9749,10 +9746,10 @@
         <v>330</v>
       </c>
       <c r="L186" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="M186" s="26" t="s">
         <v>458</v>
-      </c>
-      <c r="M186" s="26" t="s">
-        <v>459</v>
       </c>
       <c r="N186" s="26"/>
       <c r="O186" s="26"/>
@@ -9792,10 +9789,10 @@
         <v>256</v>
       </c>
       <c r="L187" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="M187" s="7" t="s">
         <v>460</v>
-      </c>
-      <c r="M187" s="7" t="s">
-        <v>461</v>
       </c>
       <c r="N187" s="26"/>
       <c r="O187" s="26"/>
@@ -9918,11 +9915,11 @@
       </c>
       <c r="J190" s="26"/>
       <c r="K190" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L190" s="26"/>
       <c r="M190" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N190" s="26">
         <v>1</v>
@@ -10010,7 +10007,7 @@
         <v>318</v>
       </c>
       <c r="M192" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N192" s="26"/>
       <c r="O192" s="26"/>
@@ -10047,11 +10044,11 @@
       </c>
       <c r="J193" s="26"/>
       <c r="K193" s="26" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L193" s="26"/>
       <c r="M193" s="26" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="N193" s="26">
         <v>4</v>
@@ -10175,16 +10172,16 @@
         <v>134</v>
       </c>
       <c r="J196" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="K196" s="36" t="s">
         <v>448</v>
       </c>
-      <c r="K196" s="36" t="s">
+      <c r="L196" s="36" t="s">
         <v>449</v>
       </c>
-      <c r="L196" s="36" t="s">
+      <c r="M196" s="7" t="s">
         <v>450</v>
-      </c>
-      <c r="M196" s="7" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="197" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -10254,10 +10251,10 @@
         <v>306</v>
       </c>
       <c r="L198" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="M198" s="7" t="s">
         <v>469</v>
-      </c>
-      <c r="M198" s="7" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="199" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -10292,7 +10289,7 @@
         <v>133</v>
       </c>
       <c r="L199" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M199" s="7" t="s">
         <v>349</v>
@@ -10330,10 +10327,10 @@
         <v>280</v>
       </c>
       <c r="L200" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="M200" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="M200" s="7" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="201" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -10368,10 +10365,10 @@
         <v>330</v>
       </c>
       <c r="L201" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="M201" s="7" t="s">
         <v>458</v>
-      </c>
-      <c r="M201" s="7" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="202" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -10552,10 +10549,10 @@
         <v>326</v>
       </c>
       <c r="L206" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="M206" s="7" t="s">
         <v>467</v>
-      </c>
-      <c r="M206" s="7" t="s">
-        <v>468</v>
       </c>
       <c r="N206" s="7"/>
       <c r="O206" s="7"/>
@@ -10634,16 +10631,16 @@
         <v>134</v>
       </c>
       <c r="J208" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="K208" s="27" t="s">
         <v>448</v>
       </c>
-      <c r="K208" s="27" t="s">
+      <c r="L208" s="27" t="s">
         <v>449</v>
       </c>
-      <c r="L208" s="27" t="s">
+      <c r="M208" s="27" t="s">
         <v>450</v>
-      </c>
-      <c r="M208" s="27" t="s">
-        <v>451</v>
       </c>
       <c r="N208" s="82"/>
       <c r="O208" s="82"/>
@@ -11311,7 +11308,7 @@
         <v>318</v>
       </c>
       <c r="M224" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N224" s="26"/>
       <c r="O224" s="26"/>
@@ -11348,11 +11345,11 @@
       </c>
       <c r="J225" s="26"/>
       <c r="K225" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L225" s="26"/>
       <c r="M225" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N225" s="26">
         <v>1</v>
@@ -11735,7 +11732,7 @@
         <v>245</v>
       </c>
       <c r="K235" s="51" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="M235" s="51" t="s">
         <v>245</v>
@@ -11885,10 +11882,10 @@
         <v>330</v>
       </c>
       <c r="L239" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="M239" s="7" t="s">
         <v>458</v>
-      </c>
-      <c r="M239" s="7" t="s">
-        <v>459</v>
       </c>
       <c r="N239" s="7"/>
       <c r="O239" s="7"/>
@@ -12158,10 +12155,10 @@
         <v>73</v>
       </c>
       <c r="L246" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M246" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M246" s="7" t="s">
-        <v>390</v>
       </c>
       <c r="N246" s="7">
         <v>2</v>
@@ -12386,10 +12383,10 @@
         <v>105</v>
       </c>
       <c r="L252" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="M252" s="7" t="s">
         <v>455</v>
-      </c>
-      <c r="M252" s="7" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="253" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -12694,10 +12691,10 @@
         <v>73</v>
       </c>
       <c r="L260" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M260" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M260" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N260" s="26"/>
       <c r="O260" s="26"/>
@@ -12730,10 +12727,10 @@
         <v>30</v>
       </c>
       <c r="I261" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="M261" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N261" s="7">
         <v>1</v>
@@ -12816,10 +12813,10 @@
         <v>330</v>
       </c>
       <c r="L263" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="M263" s="26" t="s">
         <v>458</v>
-      </c>
-      <c r="M263" s="26" t="s">
-        <v>459</v>
       </c>
       <c r="N263" s="26"/>
       <c r="O263" s="26"/>
@@ -12938,10 +12935,10 @@
         <v>256</v>
       </c>
       <c r="L266" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="M266" s="7" t="s">
         <v>463</v>
-      </c>
-      <c r="M266" s="7" t="s">
-        <v>464</v>
       </c>
       <c r="N266" s="26">
         <v>1</v>
@@ -13104,11 +13101,11 @@
       </c>
       <c r="J270" s="26"/>
       <c r="K270" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L270" s="26"/>
       <c r="M270" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N270" s="26">
         <v>1</v>
@@ -13237,7 +13234,7 @@
         <v>318</v>
       </c>
       <c r="M273" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N273" s="26"/>
       <c r="O273" s="26"/>
@@ -13387,17 +13384,17 @@
         <v>15</v>
       </c>
       <c r="I277" s="26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J277" s="26"/>
       <c r="K277" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="L277" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="L277" s="26" t="s">
+      <c r="M277" s="26" t="s">
         <v>420</v>
-      </c>
-      <c r="M277" s="26" t="s">
-        <v>421</v>
       </c>
       <c r="N277" s="26"/>
       <c r="O277" s="26"/>
@@ -13437,10 +13434,10 @@
         <v>73</v>
       </c>
       <c r="L278" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M278" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M278" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N278" s="26"/>
       <c r="O278" s="26"/>
@@ -13691,10 +13688,10 @@
         <v>105</v>
       </c>
       <c r="L284" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="M284" s="26" t="s">
         <v>455</v>
-      </c>
-      <c r="M284" s="26" t="s">
-        <v>456</v>
       </c>
       <c r="N284" s="26"/>
       <c r="O284" s="26"/>
@@ -13772,11 +13769,11 @@
       </c>
       <c r="J286" s="26"/>
       <c r="K286" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L286" s="26"/>
       <c r="M286" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N286" s="26"/>
       <c r="O286" s="26" t="s">
@@ -14150,7 +14147,7 @@
         <v>318</v>
       </c>
       <c r="M295" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N295" s="26">
         <v>1</v>
@@ -14229,7 +14226,7 @@
         <v>132</v>
       </c>
       <c r="J297" s="44" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K297" s="44"/>
       <c r="L297" s="44"/>
@@ -14272,16 +14269,16 @@
         <v>134</v>
       </c>
       <c r="J298" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="K298" s="27" t="s">
         <v>448</v>
       </c>
-      <c r="K298" s="27" t="s">
+      <c r="L298" s="27" t="s">
         <v>449</v>
       </c>
-      <c r="L298" s="27" t="s">
+      <c r="M298" s="27" t="s">
         <v>450</v>
-      </c>
-      <c r="M298" s="27" t="s">
-        <v>451</v>
       </c>
       <c r="N298" s="7"/>
       <c r="O298" s="7"/>
@@ -14526,10 +14523,10 @@
         <v>73</v>
       </c>
       <c r="L304" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M304" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M304" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N304" s="26">
         <v>2</v>
@@ -14614,10 +14611,10 @@
         <v>280</v>
       </c>
       <c r="L306" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="M306" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="M306" s="7" t="s">
-        <v>428</v>
       </c>
       <c r="N306" s="7"/>
       <c r="O306" s="26"/>
@@ -15090,10 +15087,10 @@
         <v>73</v>
       </c>
       <c r="L318" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M318" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M318" s="7" t="s">
-        <v>390</v>
       </c>
       <c r="N318" s="7"/>
       <c r="O318" s="7"/>
@@ -15326,17 +15323,17 @@
         <v>15</v>
       </c>
       <c r="I324" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J324" s="7"/>
       <c r="K324" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="L324" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="L324" s="7" t="s">
+      <c r="M324" s="7" t="s">
         <v>420</v>
-      </c>
-      <c r="M324" s="7" t="s">
-        <v>421</v>
       </c>
       <c r="N324" s="7"/>
       <c r="O324" s="7"/>
@@ -15379,7 +15376,7 @@
         <v>318</v>
       </c>
       <c r="M325" s="51" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N325" s="51"/>
       <c r="O325" s="51"/>
@@ -15497,10 +15494,10 @@
         <v>272</v>
       </c>
       <c r="K328" s="26" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="M328" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="329" spans="1:17" x14ac:dyDescent="0.35">
@@ -15615,15 +15612,15 @@
         <v>52</v>
       </c>
       <c r="I331" s="26" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J331" s="26"/>
       <c r="K331" s="26" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L331" s="26"/>
       <c r="M331" s="26" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N331" s="26">
         <v>3</v>
@@ -15664,10 +15661,10 @@
         <v>73</v>
       </c>
       <c r="L332" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="M332" s="27" t="s">
         <v>389</v>
-      </c>
-      <c r="M332" s="27" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="333" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -15705,7 +15702,7 @@
         <v>354</v>
       </c>
       <c r="N333" s="36" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="334" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -15737,10 +15734,10 @@
         <v>249</v>
       </c>
       <c r="K334" s="36" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M334" s="36" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="335" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -15925,10 +15922,10 @@
         <v>53</v>
       </c>
       <c r="K339" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M339" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N339" s="36">
         <v>1</v>
@@ -15992,16 +15989,16 @@
         <v>15</v>
       </c>
       <c r="I341" s="36" t="s">
+        <v>417</v>
+      </c>
+      <c r="K341" s="36" t="s">
         <v>418</v>
       </c>
-      <c r="K341" s="36" t="s">
+      <c r="L341" s="36" t="s">
         <v>419</v>
       </c>
-      <c r="L341" s="36" t="s">
+      <c r="M341" s="36" t="s">
         <v>420</v>
-      </c>
-      <c r="M341" s="36" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="342" spans="1:17" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -16193,10 +16190,10 @@
         <v>86</v>
       </c>
       <c r="K346" s="44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M346" s="44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N346" s="44">
         <v>2</v>
@@ -16232,11 +16229,11 @@
       </c>
       <c r="J347" s="26"/>
       <c r="K347" s="26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="L347" s="26"/>
       <c r="M347" s="26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="N347" s="26">
         <v>1</v>
@@ -16275,7 +16272,7 @@
       </c>
       <c r="J348" s="26"/>
       <c r="K348" s="26" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L348" s="26"/>
       <c r="M348" s="26" t="s">
@@ -16481,10 +16478,10 @@
         <v>53</v>
       </c>
       <c r="K353" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M353" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N353">
         <v>1</v>
@@ -16566,11 +16563,11 @@
       </c>
       <c r="J355" s="26"/>
       <c r="K355" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L355" s="26"/>
       <c r="M355" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N355" s="26">
         <v>1</v>
@@ -16609,13 +16606,13 @@
       </c>
       <c r="J356" s="26"/>
       <c r="K356" s="26" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L356" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="M356" s="26" t="s">
         <v>477</v>
-      </c>
-      <c r="M356" s="26" t="s">
-        <v>478</v>
       </c>
       <c r="N356" s="26">
         <v>4</v>
@@ -16848,10 +16845,10 @@
         <v>53</v>
       </c>
       <c r="K362" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M362" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N362" s="36">
         <v>1</v>
@@ -16891,7 +16888,7 @@
       </c>
       <c r="L363" s="51"/>
       <c r="M363" s="51" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N363" s="51">
         <v>1</v>
@@ -16974,7 +16971,7 @@
         <v>180</v>
       </c>
       <c r="L365" s="26" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M365" s="26" t="s">
         <v>177</v>
@@ -17062,7 +17059,7 @@
         <v>133</v>
       </c>
       <c r="L367" s="26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M367" s="26" t="s">
         <v>349</v>
@@ -17146,13 +17143,13 @@
         <v>14</v>
       </c>
       <c r="K369" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L369" s="44" t="s">
+        <v>476</v>
+      </c>
+      <c r="M369" s="44" t="s">
         <v>477</v>
-      </c>
-      <c r="M369" s="44" t="s">
-        <v>478</v>
       </c>
       <c r="N369" s="44">
         <v>4</v>
@@ -17392,11 +17389,11 @@
       </c>
       <c r="J375" s="26"/>
       <c r="K375" s="26" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L375" s="26"/>
       <c r="M375" s="26" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N375" s="26"/>
       <c r="O375" s="26"/>
@@ -17432,10 +17429,10 @@
         <v>86</v>
       </c>
       <c r="K376" s="44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M376" s="44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N376" s="44">
         <v>2</v>
@@ -17476,10 +17473,10 @@
         <v>16</v>
       </c>
       <c r="L377" t="s">
+        <v>485</v>
+      </c>
+      <c r="M377" t="s">
         <v>486</v>
-      </c>
-      <c r="M377" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="378" spans="1:17" x14ac:dyDescent="0.35">
@@ -17515,10 +17512,10 @@
         <v>330</v>
       </c>
       <c r="L378" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="M378" s="26" t="s">
         <v>458</v>
-      </c>
-      <c r="M378" s="26" t="s">
-        <v>459</v>
       </c>
       <c r="N378" s="26"/>
       <c r="O378" s="26"/>
@@ -17600,7 +17597,7 @@
         <v>180</v>
       </c>
       <c r="L380" s="31" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M380" s="31" t="s">
         <v>183</v>
@@ -17641,10 +17638,10 @@
         <v>280</v>
       </c>
       <c r="L381" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="M381" s="35" t="s">
         <v>427</v>
-      </c>
-      <c r="M381" s="35" t="s">
-        <v>428</v>
       </c>
       <c r="N381" s="35">
         <v>1</v>
@@ -17747,11 +17744,11 @@
       </c>
       <c r="J384" s="44"/>
       <c r="K384" s="44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L384" s="44"/>
       <c r="M384" s="44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N384" s="44">
         <v>1</v>
@@ -17834,10 +17831,10 @@
         <v>256</v>
       </c>
       <c r="L386" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="M386" s="26" t="s">
         <v>460</v>
-      </c>
-      <c r="M386" s="26" t="s">
-        <v>461</v>
       </c>
       <c r="N386" s="26"/>
       <c r="O386" s="26"/>
@@ -17959,10 +17956,10 @@
         <v>105</v>
       </c>
       <c r="L389" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="M389" s="26" t="s">
         <v>455</v>
-      </c>
-      <c r="M389" s="26" t="s">
-        <v>456</v>
       </c>
       <c r="N389" s="26"/>
       <c r="O389" s="26"/>
@@ -17999,11 +17996,11 @@
       </c>
       <c r="J390" s="26"/>
       <c r="K390" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L390" s="26"/>
       <c r="M390" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N390" s="26">
         <v>1</v>
@@ -18227,7 +18224,7 @@
         <v>302</v>
       </c>
       <c r="M396" s="35" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N396" s="35">
         <v>1</v>
@@ -18386,10 +18383,10 @@
         <v>280</v>
       </c>
       <c r="L400" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="M400" s="26" t="s">
         <v>427</v>
-      </c>
-      <c r="M400" s="26" t="s">
-        <v>428</v>
       </c>
       <c r="N400" s="26">
         <v>1</v>
@@ -18554,13 +18551,13 @@
         <v>84</v>
       </c>
       <c r="K404" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="L404" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="L404" s="28" t="s">
+      <c r="M404" s="28" t="s">
         <v>412</v>
-      </c>
-      <c r="M404" s="28" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="405" spans="1:17" x14ac:dyDescent="0.35">
@@ -18596,7 +18593,7 @@
         <v>16</v>
       </c>
       <c r="L405" s="26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M405" s="26" t="s">
         <v>16</v>
@@ -18722,11 +18719,11 @@
       </c>
       <c r="J408" s="26"/>
       <c r="K408" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L408" s="26"/>
       <c r="M408" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N408" s="26">
         <v>1</v>
@@ -18767,11 +18764,11 @@
       </c>
       <c r="J409" s="26"/>
       <c r="K409" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L409" s="26"/>
       <c r="M409" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N409" s="26">
         <v>1</v>
@@ -19621,11 +19618,11 @@
       </c>
       <c r="J430" s="26"/>
       <c r="K430" s="26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="L430" s="26"/>
       <c r="M430" s="26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N430" s="26">
         <v>1</v>
@@ -19746,13 +19743,13 @@
       </c>
       <c r="J433" s="26"/>
       <c r="K433" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="L433" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="L433" s="26" t="s">
-        <v>415</v>
-      </c>
       <c r="M433" s="26" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N433" s="26"/>
       <c r="O433" s="26"/>
@@ -20378,10 +20375,10 @@
         <v>14</v>
       </c>
       <c r="K449" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="M449" s="35" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N449" s="35">
         <v>1</v>
@@ -20492,17 +20489,17 @@
         <v>15</v>
       </c>
       <c r="I452" s="36" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J452" s="26"/>
       <c r="K452" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="L452" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="L452" s="26" t="s">
+      <c r="M452" s="26" t="s">
         <v>420</v>
-      </c>
-      <c r="M452" s="26" t="s">
-        <v>421</v>
       </c>
       <c r="N452" s="26"/>
       <c r="O452" s="26"/>
@@ -20751,13 +20748,13 @@
         <v>84</v>
       </c>
       <c r="K458" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="L458" s="27" t="s">
         <v>411</v>
       </c>
-      <c r="L458" s="27" t="s">
+      <c r="M458" s="27" t="s">
         <v>412</v>
-      </c>
-      <c r="M458" s="27" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="459" spans="1:17" x14ac:dyDescent="0.35">
@@ -21333,10 +21330,10 @@
         <v>281</v>
       </c>
       <c r="L473" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="M473" s="35" t="s">
         <v>397</v>
-      </c>
-      <c r="M473" s="35" t="s">
-        <v>398</v>
       </c>
       <c r="N473" s="35"/>
       <c r="O473" s="35"/>
@@ -21657,10 +21654,10 @@
         <v>302</v>
       </c>
       <c r="L481" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M481" s="26" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N481" s="26"/>
       <c r="O481" s="26"/>
@@ -22008,13 +22005,13 @@
         <v>53</v>
       </c>
       <c r="K490" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="L490" s="36" t="s">
         <v>396</v>
       </c>
-      <c r="L490" s="36" t="s">
+      <c r="M490" s="35" t="s">
         <v>397</v>
-      </c>
-      <c r="M490" s="35" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="491" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -22152,13 +22149,13 @@
       </c>
       <c r="J494" s="26"/>
       <c r="K494" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="L494" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="L494" s="28" t="s">
+      <c r="M494" s="28" t="s">
         <v>412</v>
-      </c>
-      <c r="M494" s="28" t="s">
-        <v>413</v>
       </c>
       <c r="N494" s="26"/>
       <c r="O494" s="26"/>
@@ -22367,7 +22364,7 @@
       </c>
       <c r="J499" s="26"/>
       <c r="K499" s="26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="L499" s="26"/>
       <c r="M499" s="26" t="s">
@@ -22453,10 +22450,10 @@
         <v>302</v>
       </c>
       <c r="L501" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="M501" s="26" t="s">
         <v>373</v>
-      </c>
-      <c r="M501" s="26" t="s">
-        <v>374</v>
       </c>
       <c r="N501" s="26"/>
     </row>
@@ -22571,13 +22568,13 @@
         <v>84</v>
       </c>
       <c r="K504" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="L504" s="28" t="s">
         <v>411</v>
       </c>
-      <c r="L504" s="28" t="s">
+      <c r="M504" s="28" t="s">
         <v>412</v>
-      </c>
-      <c r="M504" s="28" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="505" spans="1:17" x14ac:dyDescent="0.35">
@@ -23918,7 +23915,7 @@
         <v>358</v>
       </c>
       <c r="M537" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="538" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -24453,7 +24450,7 @@
       </c>
       <c r="J551" s="26"/>
       <c r="K551" s="26" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="L551" s="26"/>
       <c r="M551" s="26" t="s">
@@ -24581,7 +24578,7 @@
         <v>90</v>
       </c>
       <c r="L554" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="M554" t="s">
         <v>90</v>
@@ -25116,10 +25113,10 @@
         <v>73</v>
       </c>
       <c r="L567" s="36" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M567" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="568" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -25224,16 +25221,16 @@
         <v>44</v>
       </c>
       <c r="J570" s="36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K570" s="36" t="s">
         <v>122</v>
       </c>
       <c r="L570" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="M570" s="35" t="s">
         <v>392</v>
-      </c>
-      <c r="M570" s="35" t="s">
-        <v>393</v>
       </c>
       <c r="O570" s="35" t="s">
         <v>201</v>
@@ -25458,7 +25455,7 @@
         <v>346</v>
       </c>
       <c r="M576" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="577" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -25525,13 +25522,13 @@
         <v>53</v>
       </c>
       <c r="K578" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="L578" s="36" t="s">
         <v>396</v>
       </c>
-      <c r="L578" s="36" t="s">
+      <c r="M578" s="35" t="s">
         <v>397</v>
-      </c>
-      <c r="M578" s="35" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="579" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.35">
@@ -25893,13 +25890,13 @@
         <v>90</v>
       </c>
       <c r="K587" t="s">
+        <v>405</v>
+      </c>
+      <c r="L587" t="s">
         <v>406</v>
       </c>
-      <c r="L587" t="s">
-        <v>407</v>
-      </c>
       <c r="M587" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="O587" t="s">
         <v>205</v>
@@ -26221,10 +26218,10 @@
         <v>73</v>
       </c>
       <c r="L595" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M595" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M595" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N595" s="26"/>
       <c r="O595" s="26"/>
@@ -26431,10 +26428,10 @@
         <v>73</v>
       </c>
       <c r="L600" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M600" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M600" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N600" s="26"/>
       <c r="O600" s="26"/>
@@ -26474,7 +26471,7 @@
         <v>225</v>
       </c>
       <c r="L601" s="26" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M601" s="26" t="s">
         <v>226</v>
@@ -26751,16 +26748,16 @@
         <v>44</v>
       </c>
       <c r="J608" s="36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K608" s="36" t="s">
         <v>122</v>
       </c>
       <c r="L608" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="M608" s="35" t="s">
         <v>392</v>
-      </c>
-      <c r="M608" s="35" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="609" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -26996,7 +26993,7 @@
         <v>284</v>
       </c>
       <c r="M614" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="615" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -27110,10 +27107,10 @@
         <v>105</v>
       </c>
       <c r="L617" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="M617" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="M617" s="7" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="618" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -27286,7 +27283,7 @@
         <v>14</v>
       </c>
       <c r="J622" s="51" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K622" s="51"/>
       <c r="L622" s="51"/>
@@ -27649,10 +27646,10 @@
         <v>73</v>
       </c>
       <c r="L631" s="36" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M631" s="36" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N631" s="35">
         <v>2</v>
@@ -27946,11 +27943,11 @@
       </c>
       <c r="J639" s="36"/>
       <c r="K639" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L639" s="36"/>
       <c r="M639" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N639" s="36">
         <v>16</v>
@@ -28032,10 +28029,10 @@
         <v>73</v>
       </c>
       <c r="L641" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M641" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="M641" s="7" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="642" spans="1:14" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -28294,10 +28291,10 @@
         <v>173</v>
       </c>
       <c r="L648" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="M648" s="7" t="s">
         <v>399</v>
-      </c>
-      <c r="M648" s="7" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="649" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -28364,7 +28361,7 @@
         <v>146</v>
       </c>
       <c r="M650" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N650">
         <v>1</v>
@@ -29070,10 +29067,10 @@
         <v>73</v>
       </c>
       <c r="L668" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M668" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M668" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N668" s="26"/>
       <c r="O668" s="26"/>
@@ -29113,10 +29110,10 @@
         <v>73</v>
       </c>
       <c r="L669" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="M669" s="26" t="s">
         <v>389</v>
-      </c>
-      <c r="M669" s="26" t="s">
-        <v>390</v>
       </c>
       <c r="N669" s="26"/>
       <c r="O669" s="26"/>
@@ -29280,10 +29277,10 @@
         <v>173</v>
       </c>
       <c r="L673" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="M673" s="26" t="s">
         <v>399</v>
-      </c>
-      <c r="M673" s="26" t="s">
-        <v>400</v>
       </c>
       <c r="N673" s="26"/>
       <c r="O673" s="26"/>
@@ -29448,10 +29445,10 @@
         <v>133</v>
       </c>
       <c r="L677" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="M677" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="M677" s="7" t="s">
-        <v>382</v>
       </c>
       <c r="N677" s="7"/>
       <c r="O677" s="7" t="s">
@@ -29610,13 +29607,13 @@
       </c>
       <c r="J681" s="26"/>
       <c r="K681" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="L681" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="L681" s="26" t="s">
+      <c r="M681" s="26" t="s">
         <v>378</v>
-      </c>
-      <c r="M681" s="26" t="s">
-        <v>379</v>
       </c>
       <c r="N681" s="26"/>
       <c r="O681" s="26"/>
@@ -29770,10 +29767,10 @@
         <v>73</v>
       </c>
       <c r="L685" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="M685" s="35" t="s">
         <v>389</v>
-      </c>
-      <c r="M685" s="35" t="s">
-        <v>390</v>
       </c>
       <c r="N685" s="35"/>
       <c r="O685" s="35"/>
@@ -29890,10 +29887,10 @@
         <v>173</v>
       </c>
       <c r="L688" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="M688" s="35" t="s">
         <v>399</v>
-      </c>
-      <c r="M688" s="35" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="689" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -30009,10 +30006,10 @@
         <v>281</v>
       </c>
       <c r="L691" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="M691" s="35" t="s">
         <v>397</v>
-      </c>
-      <c r="M691" s="35" t="s">
-        <v>398</v>
       </c>
       <c r="O691" s="35" t="s">
         <v>200</v>
@@ -30520,7 +30517,7 @@
       </c>
       <c r="L703" s="7"/>
       <c r="M703" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="N703" s="7"/>
       <c r="O703" s="7"/>
@@ -31284,13 +31281,13 @@
         <v>14</v>
       </c>
       <c r="K723" s="44" t="s">
+        <v>376</v>
+      </c>
+      <c r="L723" s="44" t="s">
         <v>377</v>
       </c>
-      <c r="L723" s="44" t="s">
+      <c r="M723" s="44" t="s">
         <v>378</v>
-      </c>
-      <c r="M723" s="44" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="724" spans="1:17" x14ac:dyDescent="0.35">
@@ -31370,7 +31367,7 @@
         <v>284</v>
       </c>
       <c r="M725" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N725" s="26"/>
       <c r="O725" s="26"/>
@@ -31453,10 +31450,10 @@
         <v>302</v>
       </c>
       <c r="L727" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="M727" s="26" t="s">
         <v>373</v>
-      </c>
-      <c r="M727" s="26" t="s">
-        <v>374</v>
       </c>
       <c r="O727" s="26"/>
       <c r="P727" s="26"/>
@@ -31529,10 +31526,10 @@
         <v>73</v>
       </c>
       <c r="L729" s="36" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
       <c r="M729" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="730" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.35">
@@ -31610,7 +31607,7 @@
       <c r="K731" s="35"/>
       <c r="L731" s="35"/>
       <c r="M731" s="35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N731" s="35">
         <v>5</v>
@@ -31810,13 +31807,13 @@
       </c>
       <c r="J736" s="26"/>
       <c r="K736" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="L736" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="L736" s="26" t="s">
+      <c r="M736" s="26" t="s">
         <v>378</v>
-      </c>
-      <c r="M736" s="26" t="s">
-        <v>379</v>
       </c>
       <c r="N736" s="26"/>
       <c r="O736" s="26"/>
@@ -32020,10 +32017,10 @@
         <v>133</v>
       </c>
       <c r="L741" s="36" t="s">
+        <v>380</v>
+      </c>
+      <c r="M741" s="35" t="s">
         <v>381</v>
-      </c>
-      <c r="M741" s="35" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="742" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.35">
@@ -32519,7 +32516,7 @@
       </c>
       <c r="J754" s="26"/>
       <c r="K754" s="26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L754" s="26" t="s">
         <v>356</v>
@@ -33172,10 +33169,10 @@
         <v>73</v>
       </c>
       <c r="L771" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="M771" s="35" t="s">
         <v>389</v>
-      </c>
-      <c r="M771" s="35" t="s">
-        <v>390</v>
       </c>
       <c r="N771" s="35"/>
       <c r="O771" s="35"/>
@@ -33212,7 +33209,7 @@
       </c>
       <c r="J772" s="35"/>
       <c r="K772" s="35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L772" s="36" t="s">
         <v>356</v>
@@ -33548,13 +33545,13 @@
       </c>
       <c r="J780" s="26"/>
       <c r="K780" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="L780" s="26" t="s">
         <v>383</v>
       </c>
-      <c r="L780" s="26" t="s">
+      <c r="M780" s="26" t="s">
         <v>384</v>
-      </c>
-      <c r="M780" s="26" t="s">
-        <v>385</v>
       </c>
       <c r="N780" s="26"/>
       <c r="O780" s="26"/>
@@ -33713,11 +33710,11 @@
       </c>
       <c r="J784" s="7"/>
       <c r="K784" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L784" s="7"/>
       <c r="M784" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N784" s="7">
         <v>1</v>
@@ -33756,13 +33753,13 @@
       </c>
       <c r="J785" s="7"/>
       <c r="K785" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="L785" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="L785" s="7" t="s">
+      <c r="M785" s="7" t="s">
         <v>378</v>
-      </c>
-      <c r="M785" s="7" t="s">
-        <v>379</v>
       </c>
       <c r="N785" s="7"/>
       <c r="O785" s="7"/>
@@ -33845,7 +33842,7 @@
         <v>302</v>
       </c>
       <c r="L787" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M787" s="7" t="s">
         <v>302</v>
@@ -42359,7 +42356,7 @@
         <v>277</v>
       </c>
       <c r="M994" s="44" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N994" s="44"/>
       <c r="O994" s="44"/>
@@ -42574,7 +42571,7 @@
       </c>
       <c r="L999" s="44"/>
       <c r="M999" s="44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N999" s="44">
         <v>1</v>

</xml_diff>